<commit_message>
Inserção do confronto São Paulo X Corinthians
</commit_message>
<xml_diff>
--- a/HISTÓRICO DE CONFRONTOS/HISTÓRICO_CONFRONTOS.xlsx
+++ b/HISTÓRICO DE CONFRONTOS/HISTÓRICO_CONFRONTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janth\Desktop\Projeto das aulas\GeneticAlgorithms\HISTÓRICO DE CONFRONTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F0842-74C7-4D95-8EE5-FFA7B52B4F41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D909B699-AF05-4420-B120-D9DD745B642D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{8497CD36-2B0D-4418-85CA-FC0F9DCEB4BE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="15">
   <si>
     <t>PALMEIRAS</t>
   </si>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -251,10 +251,13 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24651CA-323D-4CE2-8FFD-6BC64671DCBC}">
   <dimension ref="A1:AN60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN10" sqref="AN10"/>
+    <sheetView tabSelected="1" topLeftCell="AD16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN35" sqref="AN35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,48 +608,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="H1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="O1" s="21" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="O1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="V1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AC1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AJ1" s="21" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="V1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AC1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AJ1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -655,10 +658,10 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
@@ -668,10 +671,10 @@
       <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="21"/>
+      <c r="K2" s="22"/>
       <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
@@ -681,10 +684,10 @@
       <c r="P2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="21"/>
+      <c r="R2" s="22"/>
       <c r="S2" s="3" t="s">
         <v>6</v>
       </c>
@@ -694,10 +697,10 @@
       <c r="W2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="21"/>
+      <c r="Y2" s="22"/>
       <c r="Z2" s="3" t="s">
         <v>6</v>
       </c>
@@ -707,10 +710,10 @@
       <c r="AD2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="21" t="s">
+      <c r="AE2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="21"/>
+      <c r="AF2" s="22"/>
       <c r="AG2" s="3" t="s">
         <v>6</v>
       </c>
@@ -720,10 +723,10 @@
       <c r="AK2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="AM2" s="21"/>
+      <c r="AM2" s="22"/>
       <c r="AN2" s="3" t="s">
         <v>6</v>
       </c>
@@ -805,13 +808,17 @@
         <v>10</v>
       </c>
       <c r="AJ3" s="20">
-        <v>38178</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="7"/>
+        <v>38137</v>
+      </c>
+      <c r="AK3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>1</v>
+      </c>
       <c r="AN3" s="19" t="s">
         <v>2</v>
       </c>
@@ -893,13 +900,17 @@
         <v>10</v>
       </c>
       <c r="AJ4" s="20">
-        <v>38270</v>
-      </c>
-      <c r="AK4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
+        <v>38249</v>
+      </c>
+      <c r="AK4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>0</v>
+      </c>
       <c r="AN4" s="19" t="s">
         <v>2</v>
       </c>
@@ -981,13 +992,17 @@
         <v>10</v>
       </c>
       <c r="AJ5" s="20">
-        <v>38280</v>
-      </c>
-      <c r="AK5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
+        <v>38480</v>
+      </c>
+      <c r="AK5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL5" s="7">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>1</v>
+      </c>
       <c r="AN5" s="19" t="s">
         <v>2</v>
       </c>
@@ -1069,13 +1084,17 @@
         <v>10</v>
       </c>
       <c r="AJ6" s="20">
-        <v>38284</v>
-      </c>
-      <c r="AK6" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL6" s="7"/>
-      <c r="AM6" s="7"/>
+        <v>38649</v>
+      </c>
+      <c r="AK6" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>1</v>
+      </c>
       <c r="AN6" s="19" t="s">
         <v>2</v>
       </c>
@@ -1157,13 +1176,17 @@
         <v>10</v>
       </c>
       <c r="AJ7" s="20">
-        <v>38445</v>
-      </c>
-      <c r="AK7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL7" s="7"/>
-      <c r="AM7" s="7"/>
+        <v>38844</v>
+      </c>
+      <c r="AK7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL7" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>1</v>
+      </c>
       <c r="AN7" s="19" t="s">
         <v>2</v>
       </c>
@@ -1245,13 +1268,17 @@
         <v>10</v>
       </c>
       <c r="AJ8" s="20">
-        <v>38550</v>
-      </c>
-      <c r="AK8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL8" s="7"/>
-      <c r="AM8" s="7"/>
+        <v>38970</v>
+      </c>
+      <c r="AK8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="7">
+        <v>0</v>
+      </c>
       <c r="AN8" s="19" t="s">
         <v>2</v>
       </c>
@@ -1333,13 +1360,17 @@
         <v>10</v>
       </c>
       <c r="AJ9" s="20">
-        <v>38647</v>
-      </c>
-      <c r="AK9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL9" s="7"/>
-      <c r="AM9" s="7"/>
+        <v>39277</v>
+      </c>
+      <c r="AK9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="7">
+        <v>1</v>
+      </c>
       <c r="AN9" s="19" t="s">
         <v>2</v>
       </c>
@@ -1421,14 +1452,18 @@
         <v>10</v>
       </c>
       <c r="AJ10" s="20">
-        <v>38809</v>
-      </c>
-      <c r="AK10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL10" s="7"/>
-      <c r="AM10" s="7"/>
-      <c r="AN10" s="19" t="s">
+        <v>39362</v>
+      </c>
+      <c r="AK10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1509,14 +1544,18 @@
         <v>10</v>
       </c>
       <c r="AJ11" s="20">
-        <v>38928</v>
-      </c>
-      <c r="AK11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL11" s="7"/>
-      <c r="AM11" s="7"/>
-      <c r="AN11" s="19" t="s">
+        <v>39985</v>
+      </c>
+      <c r="AK11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="7">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1597,13 +1636,17 @@
         <v>10</v>
       </c>
       <c r="AJ12" s="20">
-        <v>39026</v>
-      </c>
-      <c r="AK12" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL12" s="7"/>
-      <c r="AM12" s="7"/>
+        <v>40083</v>
+      </c>
+      <c r="AK12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="7">
+        <v>1</v>
+      </c>
       <c r="AN12" s="19" t="s">
         <v>2</v>
       </c>
@@ -1685,14 +1728,18 @@
         <v>10</v>
       </c>
       <c r="AJ13" s="20">
-        <v>39152</v>
-      </c>
-      <c r="AK13" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL13" s="7"/>
-      <c r="AM13" s="7"/>
-      <c r="AN13" s="19" t="s">
+        <v>40412</v>
+      </c>
+      <c r="AK13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="7">
+        <v>3</v>
+      </c>
+      <c r="AN13" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1773,14 +1820,18 @@
         <v>10</v>
       </c>
       <c r="AJ14" s="20">
-        <v>39257</v>
-      </c>
-      <c r="AK14" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="19" t="s">
+        <v>40489</v>
+      </c>
+      <c r="AK14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AN14" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1861,14 +1912,18 @@
         <v>10</v>
       </c>
       <c r="AJ15" s="20">
-        <v>39340</v>
-      </c>
-      <c r="AK15" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="7"/>
-      <c r="AN15" s="19" t="s">
+        <v>40720</v>
+      </c>
+      <c r="AK15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="7">
+        <v>5</v>
+      </c>
+      <c r="AN15" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1949,13 +2004,17 @@
         <v>10</v>
       </c>
       <c r="AJ16" s="20">
-        <v>39488</v>
-      </c>
-      <c r="AK16" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL16" s="7"/>
-      <c r="AM16" s="7"/>
+        <v>40807</v>
+      </c>
+      <c r="AK16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="7">
+        <v>0</v>
+      </c>
       <c r="AN16" s="19" t="s">
         <v>2</v>
       </c>
@@ -2037,13 +2096,17 @@
         <v>10</v>
       </c>
       <c r="AJ17" s="20">
-        <v>39600</v>
-      </c>
-      <c r="AK17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL17" s="7"/>
-      <c r="AM17" s="7"/>
+        <v>41147</v>
+      </c>
+      <c r="AK17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL17" s="7">
+        <v>2</v>
+      </c>
+      <c r="AM17" s="7">
+        <v>1</v>
+      </c>
       <c r="AN17" s="19" t="s">
         <v>2</v>
       </c>
@@ -2125,13 +2188,17 @@
         <v>10</v>
       </c>
       <c r="AJ18" s="20">
-        <v>39691</v>
-      </c>
-      <c r="AK18" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL18" s="7"/>
-      <c r="AM18" s="7"/>
+        <v>41245</v>
+      </c>
+      <c r="AK18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL18" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM18" s="7">
+        <v>1</v>
+      </c>
       <c r="AN18" s="19" t="s">
         <v>2</v>
       </c>
@@ -2213,13 +2280,17 @@
         <v>10</v>
       </c>
       <c r="AJ19" s="20">
-        <v>39873</v>
-      </c>
-      <c r="AK19" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL19" s="7"/>
-      <c r="AM19" s="7"/>
+        <v>41483</v>
+      </c>
+      <c r="AK19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL19" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="7">
+        <v>0</v>
+      </c>
       <c r="AN19" s="19" t="s">
         <v>2</v>
       </c>
@@ -2301,13 +2372,17 @@
         <v>10</v>
       </c>
       <c r="AJ20" s="20">
-        <v>40013</v>
-      </c>
-      <c r="AK20" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL20" s="7"/>
-      <c r="AM20" s="7"/>
+        <v>41560</v>
+      </c>
+      <c r="AK20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL20" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="7">
+        <v>0</v>
+      </c>
       <c r="AN20" s="19" t="s">
         <v>2</v>
       </c>
@@ -2389,13 +2464,17 @@
         <v>10</v>
       </c>
       <c r="AJ21" s="20">
-        <v>40111</v>
-      </c>
-      <c r="AK21" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL21" s="7"/>
-      <c r="AM21" s="7"/>
+        <v>41770</v>
+      </c>
+      <c r="AK21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="7">
+        <v>1</v>
+      </c>
       <c r="AN21" s="19" t="s">
         <v>2</v>
       </c>
@@ -2477,14 +2556,18 @@
         <v>10</v>
       </c>
       <c r="AJ22" s="20">
-        <v>40216</v>
-      </c>
-      <c r="AK22" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL22" s="7"/>
-      <c r="AM22" s="7"/>
-      <c r="AN22" s="19" t="s">
+        <v>41903</v>
+      </c>
+      <c r="AK22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL22" s="7">
+        <v>2</v>
+      </c>
+      <c r="AM22" s="7">
+        <v>3</v>
+      </c>
+      <c r="AN22" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2565,13 +2648,17 @@
         <v>10</v>
       </c>
       <c r="AJ23" s="20">
-        <v>40279</v>
-      </c>
-      <c r="AK23" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL23" s="7"/>
-      <c r="AM23" s="7"/>
+        <v>42225</v>
+      </c>
+      <c r="AK23" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="7">
+        <v>1</v>
+      </c>
       <c r="AN23" s="19" t="s">
         <v>2</v>
       </c>
@@ -2653,13 +2740,17 @@
         <v>10</v>
       </c>
       <c r="AJ24" s="20">
-        <v>40286</v>
-      </c>
-      <c r="AK24" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL24" s="7"/>
-      <c r="AM24" s="7"/>
+        <v>42330</v>
+      </c>
+      <c r="AK24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL24" s="7">
+        <v>6</v>
+      </c>
+      <c r="AM24" s="7">
+        <v>1</v>
+      </c>
       <c r="AN24" s="19" t="s">
         <v>2</v>
       </c>
@@ -2741,13 +2832,17 @@
         <v>10</v>
       </c>
       <c r="AJ25" s="20">
-        <v>40384</v>
-      </c>
-      <c r="AK25" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL25" s="7"/>
-      <c r="AM25" s="7"/>
+        <v>42568</v>
+      </c>
+      <c r="AK25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM25" s="7">
+        <v>1</v>
+      </c>
       <c r="AN25" s="19" t="s">
         <v>2</v>
       </c>
@@ -2829,13 +2924,17 @@
         <v>10</v>
       </c>
       <c r="AJ26" s="20">
-        <v>40468</v>
-      </c>
-      <c r="AK26" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL26" s="7"/>
-      <c r="AM26" s="7"/>
+        <v>42679</v>
+      </c>
+      <c r="AK26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL26" s="7">
+        <v>4</v>
+      </c>
+      <c r="AM26" s="7">
+        <v>0</v>
+      </c>
       <c r="AN26" s="19" t="s">
         <v>2</v>
       </c>
@@ -2917,14 +3016,18 @@
         <v>10</v>
       </c>
       <c r="AJ27" s="20">
-        <v>40573</v>
-      </c>
-      <c r="AK27" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL27" s="7"/>
-      <c r="AM27" s="7"/>
-      <c r="AN27" s="19" t="s">
+        <v>42897</v>
+      </c>
+      <c r="AK27" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL27" s="7">
+        <v>2</v>
+      </c>
+      <c r="AM27" s="7">
+        <v>3</v>
+      </c>
+      <c r="AN27" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3005,13 +3108,17 @@
         <v>10</v>
       </c>
       <c r="AJ28" s="20">
-        <v>40663</v>
-      </c>
-      <c r="AK28" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL28" s="7"/>
-      <c r="AM28" s="7"/>
+        <v>43002</v>
+      </c>
+      <c r="AK28" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL28" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM28" s="7">
+        <v>1</v>
+      </c>
       <c r="AN28" s="19" t="s">
         <v>2</v>
       </c>
@@ -3093,13 +3200,17 @@
         <v>10</v>
       </c>
       <c r="AJ29" s="20">
-        <v>40783</v>
-      </c>
-      <c r="AK29" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL29" s="7"/>
-      <c r="AM29" s="7"/>
+        <v>43302</v>
+      </c>
+      <c r="AK29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL29" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM29" s="7">
+        <v>1</v>
+      </c>
       <c r="AN29" s="19" t="s">
         <v>2</v>
       </c>
@@ -3181,13 +3292,17 @@
         <v>10</v>
       </c>
       <c r="AJ30" s="20">
-        <v>40881</v>
-      </c>
-      <c r="AK30" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL30" s="7"/>
-      <c r="AM30" s="7"/>
+        <v>43414</v>
+      </c>
+      <c r="AK30" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="7">
+        <v>1</v>
+      </c>
       <c r="AN30" s="19" t="s">
         <v>2</v>
       </c>
@@ -3269,13 +3384,17 @@
         <v>10</v>
       </c>
       <c r="AJ31" s="20">
-        <v>40986</v>
-      </c>
-      <c r="AK31" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL31" s="7"/>
-      <c r="AM31" s="7"/>
+        <v>43611</v>
+      </c>
+      <c r="AK31" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="7">
+        <v>0</v>
+      </c>
       <c r="AN31" s="19" t="s">
         <v>2</v>
       </c>
@@ -3356,19 +3475,19 @@
       <c r="AG32" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ32" s="20">
-        <v>41028</v>
-      </c>
-      <c r="AK32" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL32" s="7"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AJ32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK32" s="2">
+        <v>8</v>
+      </c>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>42113</v>
       </c>
@@ -3444,19 +3563,8 @@
       <c r="AG33" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ33" s="20">
-        <v>41070</v>
-      </c>
-      <c r="AK33" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL33" s="7"/>
-      <c r="AM33" s="7"/>
-      <c r="AN33" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>42155</v>
       </c>
@@ -3533,19 +3641,8 @@
       <c r="AG34" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ34" s="20">
-        <v>41161</v>
-      </c>
-      <c r="AK34" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL34" s="7"/>
-      <c r="AM34" s="7"/>
-      <c r="AN34" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>42253</v>
       </c>
@@ -3621,19 +3718,8 @@
       <c r="AG35" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ35" s="20">
-        <v>41308</v>
-      </c>
-      <c r="AK35" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL35" s="7"/>
-      <c r="AM35" s="7"/>
-      <c r="AN35" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>42463</v>
       </c>
@@ -3709,19 +3795,8 @@
       <c r="AG36" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ36" s="20">
-        <v>41462</v>
-      </c>
-      <c r="AK36" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL36" s="7"/>
-      <c r="AM36" s="7"/>
-      <c r="AN36" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>42533</v>
       </c>
@@ -3797,19 +3872,8 @@
       <c r="AG37" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ37" s="20">
-        <v>41549</v>
-      </c>
-      <c r="AK37" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL37" s="7"/>
-      <c r="AM37" s="7"/>
-      <c r="AN37" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>42630</v>
       </c>
@@ -3885,19 +3949,8 @@
       <c r="AG38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ38" s="20">
-        <v>41693</v>
-      </c>
-      <c r="AK38" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL38" s="7"/>
-      <c r="AM38" s="7"/>
-      <c r="AN38" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>42788</v>
       </c>
@@ -3973,19 +4026,8 @@
       <c r="AG39" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ39" s="20">
-        <v>41875</v>
-      </c>
-      <c r="AK39" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL39" s="7"/>
-      <c r="AM39" s="7"/>
-      <c r="AN39" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>42928</v>
       </c>
@@ -4062,19 +4104,8 @@
       <c r="AG40" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ40" s="20">
-        <v>41966</v>
-      </c>
-      <c r="AK40" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL40" s="7"/>
-      <c r="AM40" s="7"/>
-      <c r="AN40" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43044</v>
       </c>
@@ -4151,19 +4182,8 @@
       <c r="AG41" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ41" s="20">
-        <v>42046</v>
-      </c>
-      <c r="AK41" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL41" s="7"/>
-      <c r="AM41" s="7"/>
-      <c r="AN41" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43155</v>
       </c>
@@ -4239,19 +4259,8 @@
       <c r="AG42" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ42" s="20">
-        <v>42113</v>
-      </c>
-      <c r="AK42" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL42" s="7"/>
-      <c r="AM42" s="7"/>
-      <c r="AN42" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43190</v>
       </c>
@@ -4327,19 +4336,8 @@
       <c r="AG43" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ43" s="20">
-        <v>42158</v>
-      </c>
-      <c r="AK43" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL43" s="7"/>
-      <c r="AM43" s="7"/>
-      <c r="AN43" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43198</v>
       </c>
@@ -4415,19 +4413,8 @@
       <c r="AG44" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ44" s="20">
-        <v>42256</v>
-      </c>
-      <c r="AK44" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL44" s="7"/>
-      <c r="AM44" s="7"/>
-      <c r="AN44" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43233</v>
       </c>
@@ -4503,19 +4490,8 @@
       <c r="AG45" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ45" s="20">
-        <v>42298</v>
-      </c>
-      <c r="AK45" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL45" s="7"/>
-      <c r="AM45" s="7"/>
-      <c r="AN45" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43352</v>
       </c>
@@ -4592,19 +4568,8 @@
       <c r="AG46" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ46" s="20">
-        <v>42305</v>
-      </c>
-      <c r="AK46" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL46" s="7"/>
-      <c r="AM46" s="7"/>
-      <c r="AN46" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43498</v>
       </c>
@@ -4681,19 +4646,8 @@
       <c r="AG47" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ47" s="20">
-        <v>42456</v>
-      </c>
-      <c r="AK47" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL47" s="7"/>
-      <c r="AM47" s="7"/>
-      <c r="AN47" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -4765,19 +4719,8 @@
       <c r="AG48" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ48" s="20">
-        <v>42547</v>
-      </c>
-      <c r="AK48" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL48" s="7"/>
-      <c r="AM48" s="7"/>
-      <c r="AN48" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="H49" s="6">
         <v>42900</v>
@@ -4840,19 +4783,8 @@
       <c r="AG49" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ49" s="20">
-        <v>42656</v>
-      </c>
-      <c r="AK49" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL49" s="7"/>
-      <c r="AM49" s="7"/>
-      <c r="AN49" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="H50" s="6">
         <v>43008</v>
       </c>
@@ -4913,19 +4845,8 @@
       <c r="AG50" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ50" s="20">
-        <v>42782</v>
-      </c>
-      <c r="AK50" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL50" s="7"/>
-      <c r="AM50" s="7"/>
-      <c r="AN50" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="H51" s="6">
         <v>43135</v>
       </c>
@@ -4986,19 +4907,8 @@
       <c r="AG51" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ51" s="20">
-        <v>42925</v>
-      </c>
-      <c r="AK51" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL51" s="7"/>
-      <c r="AM51" s="7"/>
-      <c r="AN51" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="H52" s="6">
         <v>43183</v>
       </c>
@@ -5060,19 +4970,8 @@
       <c r="AG52" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ52" s="20">
-        <v>43036</v>
-      </c>
-      <c r="AK52" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL52" s="7"/>
-      <c r="AM52" s="7"/>
-      <c r="AN52" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="H53" s="6">
         <v>43186</v>
       </c>
@@ -5134,19 +5033,8 @@
       <c r="AG53" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ53" s="20">
-        <v>43149</v>
-      </c>
-      <c r="AK53" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL53" s="7"/>
-      <c r="AM53" s="7"/>
-      <c r="AN53" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="H54" s="2" t="s">
         <v>9</v>
       </c>
@@ -5203,19 +5091,8 @@
       <c r="AG54" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AJ54" s="20">
-        <v>43240</v>
-      </c>
-      <c r="AK54" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL54" s="7"/>
-      <c r="AM54" s="7"/>
-      <c r="AN54" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O55" s="2" t="s">
         <v>9</v>
       </c>
@@ -5257,19 +5134,8 @@
       <c r="AG55" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ55" s="20">
-        <v>43359</v>
-      </c>
-      <c r="AK55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL55" s="7"/>
-      <c r="AM55" s="7"/>
-      <c r="AN55" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="V56" s="20">
         <v>43534</v>
       </c>
@@ -5300,19 +5166,8 @@
       <c r="AG56" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AJ56" s="20">
-        <v>43492</v>
-      </c>
-      <c r="AK56" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL56" s="7"/>
-      <c r="AM56" s="7"/>
-      <c r="AN56" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="V57" s="20">
         <v>43555</v>
       </c>
@@ -5339,19 +5194,8 @@
       <c r="AG57" s="2">
         <v>17</v>
       </c>
-      <c r="AJ57" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK57" s="2">
-        <v>23</v>
-      </c>
-      <c r="AL57" s="2"/>
-      <c r="AM57" s="2"/>
-      <c r="AN57" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="V58" s="20">
         <v>43563</v>
       </c>
@@ -5368,7 +5212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="V59" s="20">
         <v>43628</v>
       </c>
@@ -5385,7 +5229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="V60" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>